<commit_message>
update excel templates as per the requirements
</commit_message>
<xml_diff>
--- a/fastapi/Excel/LeadZen_template.xlsx
+++ b/fastapi/Excel/LeadZen_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Project\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Analystt Project\personal\people-module\fastapi\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
-    <sheet name="Financial Advisor" sheetId="2" r:id="rId2"/>
+    <sheet name="Leads" sheetId="2" r:id="rId2"/>
     <sheet name="Disclaimer" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -26,38 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Table of Content</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Financial Advisor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    1.1 Financial Advisor Details</t>
-  </si>
-  <si>
     <t>2 Disclaimer</t>
   </si>
   <si>
-    <t>Search Details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sort Applied </t>
-  </si>
-  <si>
-    <t>Date Added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter Applied </t>
-  </si>
-  <si>
-    <t>Feed Name Is Funded</t>
-  </si>
-  <si>
-    <t>View Search results on Leadzen</t>
-  </si>
-  <si>
     <t>Other Details</t>
   </si>
   <si>
@@ -79,19 +55,22 @@
     <t>View My Export History</t>
   </si>
   <si>
-    <t>** For enquiries concerning this export request, please contact myanalyst@leadzen.ai with your Export Id XXXXX</t>
-  </si>
-  <si>
     <t>Copyright © 2021, Leadzen.Ai  All rights reserved.</t>
   </si>
   <si>
-    <t>Financial Advisor</t>
-  </si>
-  <si>
     <t>Details about the companies in your export set.</t>
   </si>
   <si>
-    <t>Prepared on Aug 09, 2021 for internal use of Kapso only</t>
+    <t>1 Leads</t>
+  </si>
+  <si>
+    <t>** For enquiries concerning this export request, please contact support@leadzen.ai with your Export Id XXXXX</t>
+  </si>
+  <si>
+    <t>Leads</t>
+  </si>
+  <si>
+    <t>For internal use only</t>
   </si>
 </sst>
 </file>
@@ -242,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -262,15 +241,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -756,18 +736,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L30"/>
+  <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:12" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:12" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
@@ -775,112 +755,79 @@
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="G4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="G8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="2" t="s">
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="J9" s="2"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G18" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G20" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G22" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G26" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
-        <v>18</v>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="G6:L6"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="G4:L4"/>
-    <mergeCell ref="G14:L14"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -893,7 +840,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,11 +849,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -920,11 +867,11 @@
       <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="10" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -938,11 +885,11 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -960,7 +907,7 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="11" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -994,19 +941,19 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
removed the girds and update text of excel templates
</commit_message>
<xml_diff>
--- a/fastapi/Excel/LeadZen_template.xlsx
+++ b/fastapi/Excel/LeadZen_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Table of Content</t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">Export Request Date </t>
   </si>
   <si>
-    <t>Export ID</t>
-  </si>
-  <si>
     <t>View My Export History</t>
   </si>
   <si>
@@ -64,20 +61,20 @@
     <t>1 Leads</t>
   </si>
   <si>
-    <t>** For enquiries concerning this export request, please contact support@leadzen.ai with your Export Id XXXXX</t>
-  </si>
-  <si>
     <t>Leads</t>
   </si>
   <si>
     <t>For internal use only</t>
+  </si>
+  <si>
+    <t>** For enquiries concerning this export request, please contact support@leadzen.ai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,13 +134,6 @@
       <i/>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,24 +214,21 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -251,7 +238,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -259,6 +246,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,20 +418,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>503775</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -460,8 +450,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="1120140"/>
-          <a:ext cx="12321540" cy="3985260"/>
+          <a:off x="388620" y="1135380"/>
+          <a:ext cx="9868755" cy="2072820"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -736,98 +726,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L23"/>
+  <dimension ref="B2:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:12" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:12" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="2:12" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+      <c r="B6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="16"/>
+      <c r="B7" s="1"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="G8" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G10" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G12" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G14" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="3" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="G4:L4"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -849,76 +930,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -934,32 +1015,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>